<commit_message>
beautifulSoup 활용 내용 추가
</commit_message>
<xml_diff>
--- a/python/2020-11-02_web_scrapping/2020년 11월 03일 네이버뮤직 Top 50.xlsx
+++ b/python/2020-11-02_web_scrapping/2020년 11월 03일 네이버뮤직 Top 50.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>순위</t>
   </si>
@@ -58,12 +58,12 @@
     <t>에잇(Prod.&amp;Feat. SUGA of BTS)</t>
   </si>
   <si>
+    <t>어떻게 이별까지 사랑하겠어, 널 사랑하는 거지</t>
+  </si>
+  <si>
     <t>눈누난나 (NUNU NANA)</t>
   </si>
   <si>
-    <t>어떻게 이별까지 사랑하겠어, 널 사랑하는 거지</t>
-  </si>
-  <si>
     <t>ALIEN</t>
   </si>
   <si>
@@ -73,12 +73,12 @@
     <t>흔들리는 꽃들 속에서 네 샴푸향이 느껴진거야</t>
   </si>
   <si>
+    <t>내 마음이 움찔했던 순간 (취향저격 그녀 X 규현)</t>
+  </si>
+  <si>
     <t>How You Like That</t>
   </si>
   <si>
-    <t>내 마음이 움찔했던 순간 (취향저격 그녀 X 규현)</t>
-  </si>
-  <si>
     <t>놓아줘 (with 태연)</t>
   </si>
   <si>
@@ -94,82 +94,82 @@
     <t>Love poem</t>
   </si>
   <si>
+    <t>너도 아는</t>
+  </si>
+  <si>
+    <t>나랑 같이 걸을래 (바른연애 길잡이 X 적재)</t>
+  </si>
+  <si>
+    <t>늦은 밤 너의 집 앞 골목길에서</t>
+  </si>
+  <si>
     <t>다시 여기 바닷가</t>
   </si>
   <si>
-    <t>나랑 같이 걸을래 (바른연애 길잡이 X 적재)</t>
-  </si>
-  <si>
-    <t>늦은 밤 너의 집 앞 골목길에서</t>
-  </si>
-  <si>
     <t>덤디덤디 (DUMDi DUMDi)</t>
   </si>
   <si>
+    <t>아로하</t>
+  </si>
+  <si>
+    <t>Blueming</t>
+  </si>
+  <si>
+    <t>살짝 설렜어 (Nonstop)</t>
+  </si>
+  <si>
+    <t>Make A Wish (Birthday Song)</t>
+  </si>
+  <si>
+    <t>오래된 노래</t>
+  </si>
+  <si>
+    <t>Bet You Wanna (Feat. Cardi B)</t>
+  </si>
+  <si>
+    <t>Bad Boy</t>
+  </si>
+  <si>
     <t>도망가</t>
   </si>
   <si>
-    <t>아로하</t>
-  </si>
-  <si>
-    <t>Blueming</t>
-  </si>
-  <si>
-    <t>살짝 설렜어 (Nonstop)</t>
-  </si>
-  <si>
-    <t>너도 아는</t>
-  </si>
-  <si>
-    <t>Make A Wish (Birthday Song)</t>
-  </si>
-  <si>
-    <t>Bet You Wanna (Feat. Cardi B)</t>
-  </si>
-  <si>
-    <t>오래된 노래</t>
-  </si>
-  <si>
-    <t>Bad Boy</t>
-  </si>
-  <si>
     <t>잠이 들어야 (Feat. 헤이즈)</t>
   </si>
   <si>
+    <t>거짓말이라도 해서 널 보고싶어</t>
+  </si>
+  <si>
+    <t>밤편지</t>
+  </si>
+  <si>
     <t>Memories</t>
   </si>
   <si>
     <t>Pretty Savage</t>
   </si>
   <si>
-    <t>거짓말이라도 해서 널 보고싶어</t>
-  </si>
-  <si>
     <t>사랑하게 될 줄 알았어</t>
   </si>
   <si>
-    <t>밤편지</t>
+    <t>너를 만나</t>
   </si>
   <si>
     <t>보라빛 밤 (pporappippam)</t>
   </si>
   <si>
-    <t>너를 만나</t>
+    <t>METEOR</t>
   </si>
   <si>
     <t>Downtown Baby</t>
   </si>
   <si>
-    <t>METEOR</t>
+    <t>모든 날, 모든 순간 (Every day, Every Moment)</t>
   </si>
   <si>
     <t>Holy (Feat. Chance The Rapper)</t>
   </si>
   <si>
-    <t>모든 날, 모든 순간 (Every day, Every Moment)</t>
-  </si>
-  <si>
-    <t>어느 날 우리</t>
+    <t>우리 사랑한 동안</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -560,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -571,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -582,7 +582,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -593,7 +593,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -604,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -615,7 +615,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -626,7 +626,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -637,7 +637,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -648,7 +648,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -659,7 +659,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -670,7 +670,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -681,7 +681,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -692,7 +692,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -703,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -714,7 +714,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -725,7 +725,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -736,7 +736,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -747,7 +747,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -758,7 +758,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -769,7 +769,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -780,7 +780,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -791,7 +791,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -802,7 +802,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -813,7 +813,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -824,7 +824,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -835,7 +835,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -846,7 +846,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -857,7 +857,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -868,7 +868,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -879,7 +879,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -890,7 +890,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -901,7 +901,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -912,7 +912,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -923,7 +923,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -934,7 +934,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -945,7 +945,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -956,7 +956,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -967,7 +967,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -978,7 +978,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -989,7 +989,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1000,7 +1000,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1011,7 +1011,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1022,7 +1022,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1033,7 +1033,7 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1044,7 +1044,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1055,7 +1055,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1066,7 +1066,7 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1077,7 +1077,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1088,6 +1088,17 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>